<commit_message>
Change cinfidence of Br6522M_CIRCLE to low
</commit_message>
<xml_diff>
--- a/raw-data/HALO/Annotation_refinement_20230922/Deconvolution_HALO_Analysis_Refined_Annotations.xlsx
+++ b/raw-data/HALO/Annotation_refinement_20230922/Deconvolution_HALO_Analysis_Refined_Annotations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/wf/wynw0sv57dbgzr24438rlw9r0000gn/T/ch.sudo.cyberduck/editor-19d85abf-0d75-4080-8976-859ccb3830cb/6e8f6e440e559c89a16f0cec021cf29e/1470510867/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/wf/wynw0sv57dbgzr24438rlw9r0000gn/T/ch.sudo.cyberduck/editor-19d85abf-0d75-4080-8976-859ccb3830cb/6e8f6e440e559c89a16f0cec021cf29e/145197966/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9894BE55-AE7E-BB45-A474-7FC7E04DB0E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01CB1E8-D1FE-8047-8444-602124441875}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READ_ME" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Column A</t>
     </r>
@@ -37,6 +38,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> = Refers to Brain number (4 digits) and area of DLPFC (Anterior=A, Middle=M, and Posterior=P)</t>
     </r>
@@ -48,6 +50,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Column B = </t>
     </r>
@@ -56,6 +59,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Color coded visual showing which </t>
     </r>
@@ -65,6 +69,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>sections belong to which slide</t>
     </r>
@@ -73,6 +78,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>. Number listed here is referring to which slide from in the series (1-8, or 1-5 for break out slides).</t>
     </r>
@@ -82,6 +88,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> A,B,C,D</t>
     </r>
@@ -90,6 +97,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> denotes which tissue section it is. A= section 1, closest to the label.</t>
     </r>
@@ -100,6 +108,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Column C = Refers to which round the section comes from. These rounds are the same as the snRNAseq rounds. You can see those rounds on the Deconvolution Plan google doc ( </t>
     </r>
@@ -110,6 +119,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://docs.google.com/document/d/1GXbV134CdPmMcSw9pPeSKeHQ8tBMCf0gLuf5Sq4RF4g/edit?usp=sharing</t>
     </r>
@@ -118,6 +128,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> ) .</t>
     </r>
@@ -129,6 +140,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Column D= </t>
     </r>
@@ -137,6 +149,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Either Star or Circle. Star=SLC17A7 (Opal 520), TMEM119 (Alexa 555), AKT3 (Opal 620), OLIG2 (Alexa 647). Circle=CLDN5 (Alexa 488), GAD1 (Opal 690), GFAP (Alexa 594), AKT3 (Opal 570). Colors in HALO are </t>
     </r>
@@ -146,6 +159,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>not</t>
     </r>
@@ -154,6 +168,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> consistent!</t>
     </r>
@@ -163,6 +178,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Each channel can be pseudo colored any color later on.</t>
     </r>
@@ -174,6 +190,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Column E</t>
     </r>
@@ -182,6 +199,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> = Average Copy intensity  for AKT3 for each section. This comes from the preanalysis algorithm. These values are from the initial analysis, not the current analysis.</t>
     </r>
@@ -193,6 +211,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Column G= </t>
     </r>
@@ -201,6 +220,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Exclusion of section from analysis. </t>
     </r>
@@ -218,6 +238,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Column J</t>
     </r>
@@ -226,6 +247,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> = Average Copy Intensity for the sections within a round. This is the copy intensity average used in the "Final" algorithms. These are values from initial analysis, these values are not reflective of current analysis.</t>
     </r>
@@ -237,6 +259,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Column K</t>
     </r>
@@ -245,6 +268,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> = Path on Neurolucida computer to the unmixed, fused image. This is not relevant for the computational side, only for the person that will be adjusting the HALO segmentation algorithms and rerunning that HALO analysis. Rounds 1 and 2 had to be redone, this is where </t>
     </r>
@@ -254,6 +278,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>RERUN</t>
     </r>
@@ -262,6 +287,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> comes from. </t>
     </r>
@@ -271,6 +297,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Reunmix</t>
     </r>
@@ -279,6 +306,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> will only be seen in rounds 2,3, and 4; this is because the original unmixing done in inform was done incorrectly.  </t>
     </r>
@@ -288,6 +316,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>RESCAN</t>
     </r>
@@ -296,6 +325,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> comes from when the initial polaris scan was blurry for that section. This section was rescanned. </t>
     </r>
@@ -305,6 +335,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Always use a RERUN, Reunmix, or RESCAN file if it exists.</t>
     </r>
@@ -316,6 +347,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Column L</t>
     </r>
@@ -324,6 +356,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> = Algorithm made and used in HALO for the "final" analysis</t>
     </r>
@@ -335,6 +368,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Column M </t>
     </r>
@@ -343,6 +377,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>= Path on Neural plasticity server to the "Final" .csv file for that section.</t>
     </r>
@@ -354,6 +389,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Column N</t>
     </r>
@@ -362,6 +398,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>= Neural plasticity file path to the raw image file. In/near the same location the fused HALO image and unmixed inform tiles can be found. The raw image in the QPTIFF in the Scan1 folder for each. The HALO and Inform information will be labeled REDO_HALO or REDO_Inform for rounds 2,3,4 and just HALO or Inform for rounds 1 and 5. REDO does not apply to the raw image EVER.</t>
     </r>
@@ -373,6 +410,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Notes:</t>
     </r>
@@ -381,6 +419,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> These algorithms will have to be adjusted. Some rounds are better than others. My goal when I was creating algorithms was to make a universal one to be used with all of the sections within one combination. After looking at the averaged average copy intensity changes for AKT3 I figured out having universal algorithms won't work. So what I did was create a preanalysis algorithm that seemed fairly okay at sementing cell types, IT IS NOT PERFECT and only 1 sections per round was assessed using the preanalysis algorithm so ADJUSTMENTS WILL BE NEEDED. Using the preanalysis algorithm for each combination was done and the average copy intesnity was taken (column D) these averages were averaged and an algorithm was made for that round (FINAL_R...) the only adjustment made in these "FINAL_R..." algorithmns is the AKT3 copy intensity. Most likely adjustments will need to be made for cell types within each round (hence MidOLIG LOWOLIG algorithmns) this takes time as multiple areas on a section need to be assessed and settings changed accordingly. This will most likely be a case by case situation where previously made algorithms may work for another section. SO before making a whole new algorithm consider what the issue is. Is it calling too many OLIGOs? Try out the adjusted oligo algorithms I made. If it doesn't solve the issue make a new one but write down the issue so you know if it is a feasible option for sections that may have the same issue. </t>
     </r>
@@ -980,6 +1019,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -987,6 +1027,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -995,31 +1036,37 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1027,6 +1074,7 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1333,26 +1381,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1584,72 +1632,72 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -1665,34 +1713,34 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
@@ -1785,51 +1833,51 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
-      <c r="X9" s="35"/>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="35"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1845,81 +1893,81 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
-      <c r="X11" s="35"/>
-      <c r="Y11" s="35"/>
-      <c r="Z11" s="35"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="32"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
-      <c r="X12" s="35"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="35"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1963,205 +2011,210 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="33"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="37"/>
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="34"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="36"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="39"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="34"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="36"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="39"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="36"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="39"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="39"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="42"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A23:L27"/>
+    <mergeCell ref="A11:Z11"/>
+    <mergeCell ref="A12:Z12"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="A15:M22"/>
     <mergeCell ref="A9:Z9"/>
     <mergeCell ref="A10:M10"/>
     <mergeCell ref="A1:M1"/>
@@ -2169,11 +2222,6 @@
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="A4:M4"/>
     <mergeCell ref="A5:Z5"/>
-    <mergeCell ref="A23:L27"/>
-    <mergeCell ref="A11:Z11"/>
-    <mergeCell ref="A12:Z12"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="A15:M22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2189,8 +2237,8 @@
   </sheetPr>
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3529,7 +3577,7 @@
         <v>44</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="J31" s="43">
         <f>AVERAGE(E31:E34)</f>

</xml_diff>